<commit_message>
Added data for ProvarCache
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="141">
   <si>
     <t>Item Number</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>a345f000000uK0KAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-4EFMG</t>
+  </si>
+  <si>
+    <t>a345f000000uL5gAAE</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +501,18 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -625,7 +643,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -663,11 +681,14 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -691,8 +712,10 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="21" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="10" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="22" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="23" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="11" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1127,9 +1150,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.73828125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.26953125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.30859375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.6484375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1151,13 +1174,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Test Plans/Try TestCycle
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="181">
   <si>
     <t>Item Number</t>
   </si>
@@ -571,6 +571,18 @@
   </si>
   <si>
     <t>a345f000000uLVFAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-JIW68</t>
+  </si>
+  <si>
+    <t>a345f000000uMMjAAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-NO6BD</t>
+  </si>
+  <si>
+    <t>a345f000000uMMoAAM</t>
   </si>
 </sst>
 </file>
@@ -581,7 +593,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="68" x14ac:knownFonts="1">
+  <fonts count="72" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +621,30 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1003,7 +1039,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1107,11 +1143,17 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1179,8 +1221,12 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="63" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="64" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="65" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="67" fillId="0" borderId="32" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="66" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="67" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="68" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="69" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="71" fillId="0" borderId="34" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1615,9 +1661,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.16015625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.34375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.30078125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1639,13 +1685,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>